<commit_message>
Updated Task Schedule with completed tasks.  Man, I need to set up Trello/GitHub Issue Tracking
</commit_message>
<xml_diff>
--- a/Design Documents/FamilyShare Task Schedule.xlsx
+++ b/Design Documents/FamilyShare Task Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottnicholes/Documents/FamilyShare/FamilyShare_Master_Project/Design Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2846ED-E7C2-E445-8CA2-071C892EC8FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC61E945-07C4-8B42-97E8-830039F8BC66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16000" xr2:uid="{75145E67-4060-2A45-9217-CC1CABBA951C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="82">
   <si>
     <t xml:space="preserve">   - Provide ability to view an Ancestor's Temple Work (4 Hours)</t>
   </si>
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C06239-2855-7A4A-AF13-AB950A38A297}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1273,6 +1273,9 @@
       <c r="J31" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="K31" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="2" t="s">
@@ -1499,15 +1502,18 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="B43:I43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B36:I36"/>
-    <mergeCell ref="B37:I37"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="B39:I39"/>
-    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B22:I22"/>
     <mergeCell ref="B35:I35"/>
     <mergeCell ref="B24:I24"/>
     <mergeCell ref="B25:I25"/>
@@ -1520,18 +1526,15 @@
     <mergeCell ref="B32:I32"/>
     <mergeCell ref="B33:I33"/>
     <mergeCell ref="B34:I34"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="B37:I37"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B39:I39"/>
+    <mergeCell ref="B40:I40"/>
   </mergeCells>
   <conditionalFormatting sqref="J36 J38:J40">
     <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="Week 1">

</xml_diff>

<commit_message>
Committing changes to Task Schedule and adding an gitignore file
</commit_message>
<xml_diff>
--- a/Design Documents/FamilyShare Task Schedule.xlsx
+++ b/Design Documents/FamilyShare Task Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottnicholes/Documents/FamilyShare/FamilyShare_Master_Project/Design Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC61E945-07C4-8B42-97E8-830039F8BC66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7928882A-B630-0441-A10B-F28A0BB1039A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16000" xr2:uid="{75145E67-4060-2A45-9217-CC1CABBA951C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="82">
   <si>
     <t xml:space="preserve">   - Provide ability to view an Ancestor's Temple Work (4 Hours)</t>
   </si>
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C06239-2855-7A4A-AF13-AB950A38A297}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1294,6 +1294,9 @@
       <c r="J32" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="K32" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="2" t="s">
@@ -1347,6 +1350,9 @@
       <c r="I35" s="4"/>
       <c r="J35" s="2" t="s">
         <v>61</v>
+      </c>
+      <c r="K35" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1432,6 +1438,9 @@
       <c r="J40" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="K40" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="2" t="s">
@@ -1485,6 +1494,9 @@
       <c r="I43" s="4"/>
       <c r="J43" s="2" t="s">
         <v>57</v>
+      </c>
+      <c r="K43" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:11">

</xml_diff>